<commit_message>
algunos agregados menores con numpy y al autografico
</commit_message>
<xml_diff>
--- a/excel_info/coches_por_cabecera.xlsx
+++ b/excel_info/coches_por_cabecera.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\repuestos01\Documents\Programas\auto_plot\excel_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABD378D-BDB5-4040-8688-5959ED34BF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFBD1D1-E509-405F-ABAF-FCF0639FE668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Cabecera</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>ESISA</t>
+  </si>
+  <si>
+    <t>MARY GO</t>
+  </si>
+  <si>
+    <t>EL PUENTE</t>
   </si>
 </sst>
 </file>
@@ -126,13 +132,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -146,11 +159,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BD81DD8-E4DF-42B4-8E83-B6F135C5B2E3}" name="Tabla1" displayName="Tabla1" ref="A1:B21" totalsRowShown="0">
-  <autoFilter ref="A1:B21" xr:uid="{7BD81DD8-E4DF-42B4-8E83-B6F135C5B2E3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BD81DD8-E4DF-42B4-8E83-B6F135C5B2E3}" name="Tabla1" displayName="Tabla1" ref="A1:B23" totalsRowShown="0">
+  <autoFilter ref="A1:B23" xr:uid="{7BD81DD8-E4DF-42B4-8E83-B6F135C5B2E3}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7306DC30-5269-403F-B930-1A5CE335CC79}" name="Cabecera"/>
-    <tableColumn id="2" xr3:uid="{D853C160-E5DF-4CB2-B6AA-743A12966CF6}" name="CantidadCoches"/>
+    <tableColumn id="2" xr3:uid="{D853C160-E5DF-4CB2-B6AA-743A12966CF6}" name="CantidadCoches" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -419,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +456,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>140</v>
       </c>
     </row>
@@ -451,7 +464,7 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>242</v>
       </c>
     </row>
@@ -459,7 +472,7 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>111</v>
       </c>
     </row>
@@ -467,7 +480,7 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>215</v>
       </c>
     </row>
@@ -475,7 +488,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>192</v>
       </c>
     </row>
@@ -483,7 +496,7 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>85</v>
       </c>
     </row>
@@ -491,7 +504,7 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>91</v>
       </c>
     </row>
@@ -499,7 +512,7 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>1015</v>
       </c>
     </row>
@@ -507,7 +520,7 @@
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>85</v>
       </c>
     </row>
@@ -515,7 +528,7 @@
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>227</v>
       </c>
     </row>
@@ -523,7 +536,7 @@
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>117</v>
       </c>
     </row>
@@ -531,7 +544,7 @@
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>111</v>
       </c>
     </row>
@@ -539,7 +552,7 @@
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>310</v>
       </c>
     </row>
@@ -547,7 +560,7 @@
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>137</v>
       </c>
     </row>
@@ -555,7 +568,7 @@
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>201</v>
       </c>
     </row>
@@ -563,7 +576,7 @@
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>192</v>
       </c>
     </row>
@@ -571,7 +584,7 @@
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>144</v>
       </c>
     </row>
@@ -579,7 +592,7 @@
       <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>74</v>
       </c>
     </row>
@@ -587,7 +600,7 @@
       <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>51</v>
       </c>
     </row>
@@ -595,8 +608,24 @@
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>